<commit_message>
Fixing the last developmetns
</commit_message>
<xml_diff>
--- a/adjustmetns/baseForestdjustmens.xlsx
+++ b/adjustmetns/baseForestdjustmens.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="IDN" sheetId="1" r:id="rId1"/>
@@ -943,10 +943,10 @@
   <dimension ref="A1:AM48"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="R2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="1" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:AM1"/>
+      <selection pane="bottomRight" activeCell="Y34" sqref="Y34:AM35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2552,64 +2552,64 @@
         <v>363810.83470000001</v>
       </c>
       <c r="Y26" s="1">
-        <f t="shared" ref="Y26:AM26" si="6">$X$26*Y$19/$X$19</f>
-        <v>374725.15552434477</v>
+        <f>X26</f>
+        <v>363810.83470000001</v>
       </c>
       <c r="Z26" s="1">
-        <f t="shared" si="6"/>
-        <v>290851.94404091733</v>
+        <f>$Y$26*Z$19/$Y$19*(1/3)+(2/3)*$Y$26</f>
+        <v>336667.4002575326</v>
       </c>
       <c r="AA26" s="1">
-        <f t="shared" si="6"/>
-        <v>131564.14471657577</v>
+        <f t="shared" ref="AA26:AM26" si="6">$Y$26*AA$19/$Y$19*(1/3)+(2/3)*$Y$26</f>
+        <v>285117.95005793608</v>
       </c>
       <c r="AB26" s="1">
         <f t="shared" si="6"/>
-        <v>132879.79383926271</v>
+        <v>285543.72647783626</v>
       </c>
       <c r="AC26" s="1">
         <f t="shared" si="6"/>
-        <v>134208.59657221258</v>
+        <v>285973.75972958462</v>
       </c>
       <c r="AD26" s="1">
         <f t="shared" si="6"/>
-        <v>135550.68591422139</v>
+        <v>286408.09285486321</v>
       </c>
       <c r="AE26" s="1">
         <f t="shared" si="6"/>
-        <v>136906.18810360983</v>
+        <v>286846.766707498</v>
       </c>
       <c r="AF26" s="1">
         <f t="shared" si="6"/>
-        <v>138275.24466730061</v>
+        <v>287289.82708908257</v>
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="6"/>
-        <v>139658.01268433646</v>
+        <v>287737.32483425911</v>
       </c>
       <c r="AH26" s="1">
         <f t="shared" si="6"/>
-        <v>141054.57673898133</v>
+        <v>288189.28731657629</v>
       </c>
       <c r="AI26" s="1">
         <f t="shared" si="6"/>
-        <v>142465.13955382406</v>
+        <v>288645.78014205047</v>
       </c>
       <c r="AJ26" s="1">
         <f t="shared" si="6"/>
-        <v>143889.7719116442</v>
+        <v>289106.82621773041</v>
       </c>
       <c r="AK26" s="1">
         <f t="shared" si="6"/>
-        <v>145328.68218574242</v>
+        <v>289572.49297834199</v>
       </c>
       <c r="AL26" s="1">
         <f t="shared" si="6"/>
-        <v>146781.96795429394</v>
+        <v>290042.81200258306</v>
       </c>
       <c r="AM26" s="1">
         <f t="shared" si="6"/>
-        <v>148249.79639635611</v>
+        <v>290517.83739370899</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
@@ -2705,64 +2705,64 @@
         <v>363810.83470000001</v>
       </c>
       <c r="Y27" s="1">
-        <f t="shared" ref="Y27:AM27" si="8">$X$27*Y$19/$X$19</f>
-        <v>374725.15552434477</v>
+        <f>X27</f>
+        <v>363810.83470000001</v>
       </c>
       <c r="Z27" s="1">
-        <f t="shared" si="8"/>
-        <v>290851.94404091733</v>
+        <f>$Y$27*Z$19/$Y$19*(1/3)+(2/3)*$Y$27</f>
+        <v>336667.4002575326</v>
       </c>
       <c r="AA27" s="1">
-        <f t="shared" si="8"/>
-        <v>131564.14471657577</v>
+        <f t="shared" ref="AA27:AM27" si="8">$Y$27*AA$19/$Y$19*(1/3)+(2/3)*$Y$27</f>
+        <v>285117.95005793608</v>
       </c>
       <c r="AB27" s="1">
         <f t="shared" si="8"/>
-        <v>132879.79383926271</v>
+        <v>285543.72647783626</v>
       </c>
       <c r="AC27" s="1">
         <f t="shared" si="8"/>
-        <v>134208.59657221258</v>
+        <v>285973.75972958462</v>
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="8"/>
-        <v>135550.68591422139</v>
+        <v>286408.09285486321</v>
       </c>
       <c r="AE27" s="1">
         <f t="shared" si="8"/>
-        <v>136906.18810360983</v>
+        <v>286846.766707498</v>
       </c>
       <c r="AF27" s="1">
         <f t="shared" si="8"/>
-        <v>138275.24466730061</v>
+        <v>287289.82708908257</v>
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="8"/>
-        <v>139658.01268433646</v>
+        <v>287737.32483425911</v>
       </c>
       <c r="AH27" s="1">
         <f t="shared" si="8"/>
-        <v>141054.57673898133</v>
+        <v>288189.28731657629</v>
       </c>
       <c r="AI27" s="1">
         <f t="shared" si="8"/>
-        <v>142465.13955382406</v>
+        <v>288645.78014205047</v>
       </c>
       <c r="AJ27" s="1">
         <f t="shared" si="8"/>
-        <v>143889.7719116442</v>
+        <v>289106.82621773041</v>
       </c>
       <c r="AK27" s="1">
         <f t="shared" si="8"/>
-        <v>145328.68218574242</v>
+        <v>289572.49297834199</v>
       </c>
       <c r="AL27" s="1">
         <f t="shared" si="8"/>
-        <v>146781.96795429394</v>
+        <v>290042.81200258306</v>
       </c>
       <c r="AM27" s="1">
         <f t="shared" si="8"/>
-        <v>148249.79639635611</v>
+        <v>290517.83739370899</v>
       </c>
     </row>
     <row r="29" spans="1:39" ht="23.25" x14ac:dyDescent="0.35">
@@ -3115,8 +3115,8 @@
         <v>634255.83200000005</v>
       </c>
       <c r="Y34" s="1">
-        <f>$X34*(1-Y$19/$X$30)</f>
-        <v>632379.27173057396</v>
+        <f>X34</f>
+        <v>634255.83200000005</v>
       </c>
       <c r="Z34" s="1">
         <f>$X34*(1-Z$19/$X$30)</f>
@@ -3265,8 +3265,8 @@
         <v>634255.83200000005</v>
       </c>
       <c r="Y35" s="1">
-        <f>$X35*(1-Y$19/$X$30)</f>
-        <v>632379.27173057396</v>
+        <f>X35</f>
+        <v>634255.83200000005</v>
       </c>
       <c r="Z35" s="1">
         <f>$X35*(1-Z$19/$X$30)</f>
@@ -3421,63 +3421,63 @@
       </c>
       <c r="Y38">
         <f t="shared" si="18"/>
-        <v>1007104.4272549187</v>
+        <v>998066.66670000006</v>
       </c>
       <c r="Z38">
         <f t="shared" si="18"/>
-        <v>923651.23864430515</v>
+        <v>969466.69486092043</v>
       </c>
       <c r="AA38">
         <f t="shared" si="18"/>
-        <v>765161.12570746569</v>
+        <v>918714.93104882608</v>
       </c>
       <c r="AB38">
         <f t="shared" si="18"/>
-        <v>766470.18628162378</v>
+        <v>919134.11892019736</v>
       </c>
       <c r="AC38">
         <f t="shared" si="18"/>
-        <v>767792.3345949871</v>
+        <v>919557.49775235914</v>
       </c>
       <c r="AD38">
         <f t="shared" si="18"/>
-        <v>769127.70298031578</v>
+        <v>919985.10992095759</v>
       </c>
       <c r="AE38">
         <f t="shared" si="18"/>
-        <v>770476.41704375041</v>
+        <v>920416.99564763857</v>
       </c>
       <c r="AF38">
         <f t="shared" si="18"/>
-        <v>771838.61760347104</v>
+        <v>920853.200025253</v>
       </c>
       <c r="AG38">
         <f t="shared" si="18"/>
-        <v>773214.46095189475</v>
+        <v>921293.77310181747</v>
       </c>
       <c r="AH38">
         <f t="shared" si="18"/>
-        <v>774604.03124970198</v>
+        <v>921738.74182729702</v>
       </c>
       <c r="AI38">
         <f t="shared" si="18"/>
-        <v>776007.53020428133</v>
+        <v>922188.17079250771</v>
       </c>
       <c r="AJ38">
         <f t="shared" si="18"/>
-        <v>777425.02824394358</v>
+        <v>922642.08255002985</v>
       </c>
       <c r="AK38">
         <f t="shared" si="18"/>
-        <v>778856.73269849166</v>
+        <v>923100.54349109123</v>
       </c>
       <c r="AL38">
         <f t="shared" si="18"/>
-        <v>780302.74065744539</v>
+        <v>923563.58470573451</v>
       </c>
       <c r="AM38">
         <f t="shared" si="18"/>
-        <v>781763.21846265788</v>
+        <v>924031.2594600108</v>
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
@@ -3571,63 +3571,63 @@
       </c>
       <c r="Y39">
         <f t="shared" si="19"/>
-        <v>1007104.4272549187</v>
+        <v>998066.66670000006</v>
       </c>
       <c r="Z39">
         <f t="shared" si="19"/>
-        <v>923651.23864430515</v>
+        <v>969466.69486092043</v>
       </c>
       <c r="AA39">
         <f t="shared" si="19"/>
-        <v>765161.12570746569</v>
+        <v>918714.93104882608</v>
       </c>
       <c r="AB39">
         <f t="shared" si="19"/>
-        <v>766470.18628162378</v>
+        <v>919134.11892019736</v>
       </c>
       <c r="AC39">
         <f t="shared" si="19"/>
-        <v>767792.3345949871</v>
+        <v>919557.49775235914</v>
       </c>
       <c r="AD39">
         <f t="shared" si="19"/>
-        <v>769127.70298031578</v>
+        <v>919985.10992095759</v>
       </c>
       <c r="AE39">
         <f t="shared" si="19"/>
-        <v>770476.41704375041</v>
+        <v>920416.99564763857</v>
       </c>
       <c r="AF39">
         <f t="shared" si="19"/>
-        <v>771838.61760347104</v>
+        <v>920853.200025253</v>
       </c>
       <c r="AG39">
         <f t="shared" si="19"/>
-        <v>773214.46095189475</v>
+        <v>921293.77310181747</v>
       </c>
       <c r="AH39">
         <f t="shared" si="19"/>
-        <v>774604.03124970198</v>
+        <v>921738.74182729702</v>
       </c>
       <c r="AI39">
         <f t="shared" si="19"/>
-        <v>776007.53020428133</v>
+        <v>922188.17079250771</v>
       </c>
       <c r="AJ39">
         <f t="shared" si="19"/>
-        <v>777425.02824394358</v>
+        <v>922642.08255002985</v>
       </c>
       <c r="AK39">
         <f t="shared" si="19"/>
-        <v>778856.73269849166</v>
+        <v>923100.54349109123</v>
       </c>
       <c r="AL39">
         <f t="shared" si="19"/>
-        <v>780302.74065744539</v>
+        <v>923563.58470573451</v>
       </c>
       <c r="AM39">
         <f t="shared" si="19"/>
-        <v>781763.21846265788</v>
+        <v>924031.2594600108</v>
       </c>
     </row>
     <row r="42" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
@@ -3734,63 +3734,63 @@
       </c>
       <c r="Y43">
         <f t="shared" si="21"/>
-        <v>374725.15552434477</v>
+        <v>363810.83470000001</v>
       </c>
       <c r="Z43">
         <f t="shared" si="21"/>
-        <v>290851.94404091733</v>
+        <v>336667.4002575326</v>
       </c>
       <c r="AA43">
         <f t="shared" si="21"/>
-        <v>131564.14471657577</v>
+        <v>285117.95005793608</v>
       </c>
       <c r="AB43">
         <f t="shared" si="21"/>
-        <v>132879.79383926271</v>
+        <v>285543.72647783626</v>
       </c>
       <c r="AC43">
         <f t="shared" si="21"/>
-        <v>134208.59657221258</v>
+        <v>285973.75972958462</v>
       </c>
       <c r="AD43">
         <f t="shared" si="21"/>
-        <v>135550.68591422139</v>
+        <v>286408.09285486321</v>
       </c>
       <c r="AE43">
         <f t="shared" si="21"/>
-        <v>136906.18810360983</v>
+        <v>286846.766707498</v>
       </c>
       <c r="AF43">
         <f t="shared" si="21"/>
-        <v>138275.24466730061</v>
+        <v>287289.82708908257</v>
       </c>
       <c r="AG43">
         <f t="shared" si="21"/>
-        <v>139658.01268433646</v>
+        <v>287737.32483425911</v>
       </c>
       <c r="AH43">
         <f t="shared" si="21"/>
-        <v>141054.57673898133</v>
+        <v>288189.28731657629</v>
       </c>
       <c r="AI43">
         <f t="shared" si="21"/>
-        <v>142465.13955382406</v>
+        <v>288645.78014205047</v>
       </c>
       <c r="AJ43">
         <f t="shared" si="21"/>
-        <v>143889.7719116442</v>
+        <v>289106.82621773041</v>
       </c>
       <c r="AK43">
         <f t="shared" si="21"/>
-        <v>145328.68218574242</v>
+        <v>289572.49297834199</v>
       </c>
       <c r="AL43">
         <f t="shared" si="21"/>
-        <v>146781.96795429394</v>
+        <v>290042.81200258306</v>
       </c>
       <c r="AM43">
         <f t="shared" si="21"/>
-        <v>148249.79639635611</v>
+        <v>290517.83739370899</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
@@ -3892,63 +3892,63 @@
       </c>
       <c r="Y44">
         <f t="shared" si="23"/>
-        <v>374725.15552434477</v>
+        <v>363810.83470000001</v>
       </c>
       <c r="Z44">
         <f t="shared" si="23"/>
-        <v>290851.94404091733</v>
+        <v>336667.4002575326</v>
       </c>
       <c r="AA44">
         <f t="shared" si="23"/>
-        <v>131564.14471657577</v>
+        <v>285117.95005793608</v>
       </c>
       <c r="AB44">
         <f t="shared" si="23"/>
-        <v>132879.79383926271</v>
+        <v>285543.72647783626</v>
       </c>
       <c r="AC44">
         <f t="shared" si="23"/>
-        <v>134208.59657221258</v>
+        <v>285973.75972958462</v>
       </c>
       <c r="AD44">
         <f t="shared" si="23"/>
-        <v>135550.68591422139</v>
+        <v>286408.09285486321</v>
       </c>
       <c r="AE44">
         <f t="shared" si="23"/>
-        <v>136906.18810360983</v>
+        <v>286846.766707498</v>
       </c>
       <c r="AF44">
         <f t="shared" si="23"/>
-        <v>138275.24466730061</v>
+        <v>287289.82708908257</v>
       </c>
       <c r="AG44">
         <f t="shared" si="23"/>
-        <v>139658.01268433646</v>
+        <v>287737.32483425911</v>
       </c>
       <c r="AH44">
         <f t="shared" si="23"/>
-        <v>141054.57673898133</v>
+        <v>288189.28731657629</v>
       </c>
       <c r="AI44">
         <f t="shared" si="23"/>
-        <v>142465.13955382406</v>
+        <v>288645.78014205047</v>
       </c>
       <c r="AJ44">
         <f t="shared" si="23"/>
-        <v>143889.7719116442</v>
+        <v>289106.82621773041</v>
       </c>
       <c r="AK44">
         <f t="shared" si="23"/>
-        <v>145328.68218574242</v>
+        <v>289572.49297834199</v>
       </c>
       <c r="AL44">
         <f t="shared" si="23"/>
-        <v>146781.96795429394</v>
+        <v>290042.81200258306</v>
       </c>
       <c r="AM44">
         <f t="shared" si="23"/>
-        <v>148249.79639635611</v>
+        <v>290517.83739370899</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
@@ -4050,7 +4050,7 @@
       </c>
       <c r="Y45">
         <f t="shared" si="25"/>
-        <v>632379.27173057396</v>
+        <v>634255.83200000005</v>
       </c>
       <c r="Z45">
         <f t="shared" si="25"/>
@@ -4208,7 +4208,7 @@
       </c>
       <c r="Y46">
         <f t="shared" si="27"/>
-        <v>632379.27173057396</v>
+        <v>634255.83200000005</v>
       </c>
       <c r="Z46">
         <f t="shared" si="27"/>
@@ -4366,63 +4366,63 @@
       </c>
       <c r="Y47">
         <f t="shared" si="29"/>
-        <v>1007104.4272549187</v>
+        <v>998066.66670000006</v>
       </c>
       <c r="Z47">
         <f t="shared" si="29"/>
-        <v>923651.23864430515</v>
+        <v>969466.69486092043</v>
       </c>
       <c r="AA47">
         <f t="shared" si="29"/>
-        <v>765161.12570746569</v>
+        <v>918714.93104882608</v>
       </c>
       <c r="AB47">
         <f t="shared" si="29"/>
-        <v>766470.18628162378</v>
+        <v>919134.11892019736</v>
       </c>
       <c r="AC47">
         <f t="shared" si="29"/>
-        <v>767792.3345949871</v>
+        <v>919557.49775235914</v>
       </c>
       <c r="AD47">
         <f t="shared" si="29"/>
-        <v>769127.70298031578</v>
+        <v>919985.10992095759</v>
       </c>
       <c r="AE47">
         <f t="shared" si="29"/>
-        <v>770476.41704375041</v>
+        <v>920416.99564763857</v>
       </c>
       <c r="AF47">
         <f t="shared" si="29"/>
-        <v>771838.61760347104</v>
+        <v>920853.200025253</v>
       </c>
       <c r="AG47">
         <f t="shared" si="29"/>
-        <v>773214.46095189475</v>
+        <v>921293.77310181747</v>
       </c>
       <c r="AH47">
         <f t="shared" si="29"/>
-        <v>774604.03124970198</v>
+        <v>921738.74182729702</v>
       </c>
       <c r="AI47">
         <f t="shared" si="29"/>
-        <v>776007.53020428133</v>
+        <v>922188.17079250771</v>
       </c>
       <c r="AJ47">
         <f t="shared" si="29"/>
-        <v>777425.02824394358</v>
+        <v>922642.08255002985</v>
       </c>
       <c r="AK47">
         <f t="shared" si="29"/>
-        <v>778856.73269849166</v>
+        <v>923100.54349109123</v>
       </c>
       <c r="AL47">
         <f t="shared" si="29"/>
-        <v>780302.74065744539</v>
+        <v>923563.58470573451</v>
       </c>
       <c r="AM47">
         <f t="shared" si="29"/>
-        <v>781763.21846265788</v>
+        <v>924031.2594600108</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
@@ -4524,63 +4524,63 @@
       </c>
       <c r="Y48">
         <f t="shared" si="31"/>
-        <v>1007104.4272549187</v>
+        <v>998066.66670000006</v>
       </c>
       <c r="Z48">
         <f t="shared" si="31"/>
-        <v>923651.23864430515</v>
+        <v>969466.69486092043</v>
       </c>
       <c r="AA48">
         <f t="shared" si="31"/>
-        <v>765161.12570746569</v>
+        <v>918714.93104882608</v>
       </c>
       <c r="AB48">
         <f t="shared" si="31"/>
-        <v>766470.18628162378</v>
+        <v>919134.11892019736</v>
       </c>
       <c r="AC48">
         <f t="shared" si="31"/>
-        <v>767792.3345949871</v>
+        <v>919557.49775235914</v>
       </c>
       <c r="AD48">
         <f t="shared" si="31"/>
-        <v>769127.70298031578</v>
+        <v>919985.10992095759</v>
       </c>
       <c r="AE48">
         <f t="shared" si="31"/>
-        <v>770476.41704375041</v>
+        <v>920416.99564763857</v>
       </c>
       <c r="AF48">
         <f t="shared" si="31"/>
-        <v>771838.61760347104</v>
+        <v>920853.200025253</v>
       </c>
       <c r="AG48">
         <f t="shared" si="31"/>
-        <v>773214.46095189475</v>
+        <v>921293.77310181747</v>
       </c>
       <c r="AH48">
         <f t="shared" si="31"/>
-        <v>774604.03124970198</v>
+        <v>921738.74182729702</v>
       </c>
       <c r="AI48">
         <f t="shared" si="31"/>
-        <v>776007.53020428133</v>
+        <v>922188.17079250771</v>
       </c>
       <c r="AJ48">
         <f t="shared" si="31"/>
-        <v>777425.02824394358</v>
+        <v>922642.08255002985</v>
       </c>
       <c r="AK48">
         <f t="shared" si="31"/>
-        <v>778856.73269849166</v>
+        <v>923100.54349109123</v>
       </c>
       <c r="AL48">
         <f t="shared" si="31"/>
-        <v>780302.74065744539</v>
+        <v>923563.58470573451</v>
       </c>
       <c r="AM48">
         <f t="shared" si="31"/>
-        <v>781763.21846265788</v>
+        <v>924031.2594600108</v>
       </c>
     </row>
   </sheetData>
@@ -4592,11 +4592,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="S11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="Z26" sqref="Z26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6202,64 +6202,64 @@
         <v>24614.9895</v>
       </c>
       <c r="Y26" s="1">
-        <f t="shared" ref="Y26:AM26" si="5">$X$26*Y$19/$X$19</f>
-        <v>25353.330081113923</v>
+        <f>X26</f>
+        <v>24614.9895</v>
       </c>
       <c r="Z26" s="1">
-        <f t="shared" si="5"/>
-        <v>10669.374094537761</v>
+        <f>$Y$26*Z$19/$Y$19*(1/3)+(2/3)*$Y$26</f>
+        <v>19862.87973412115</v>
       </c>
       <c r="AA26" s="1">
-        <f t="shared" si="5"/>
-        <v>4405.66840931554</v>
+        <f t="shared" ref="AA26:AM26" si="5">$Y$26*AA$19/$Y$19*(1/3)+(2/3)*$Y$26</f>
+        <v>17835.781792357582</v>
       </c>
       <c r="AB26" s="1">
         <f t="shared" si="5"/>
-        <v>4427.6967982722335</v>
+        <v>17842.910751500702</v>
       </c>
       <c r="AC26" s="1">
         <f t="shared" si="5"/>
-        <v>4449.0263974915642</v>
+        <v>17849.813564124568</v>
       </c>
       <c r="AD26" s="1">
         <f t="shared" si="5"/>
-        <v>4472.4035508416664</v>
+        <v>17857.379018477266</v>
       </c>
       <c r="AE26" s="1">
         <f t="shared" si="5"/>
-        <v>4494.6359459893101</v>
+        <v>17864.573999325519</v>
       </c>
       <c r="AF26" s="1">
         <f t="shared" si="5"/>
-        <v>4517.0324832400929</v>
+        <v>17871.822100824094</v>
       </c>
       <c r="AG26" s="1">
         <f t="shared" si="5"/>
-        <v>4539.5725058869148</v>
+        <v>17879.116637925745</v>
       </c>
       <c r="AH26" s="1">
         <f t="shared" si="5"/>
-        <v>4562.2431689469986</v>
+        <v>17886.45345366023</v>
       </c>
       <c r="AI26" s="1">
         <f t="shared" si="5"/>
-        <v>4585.0374436029961</v>
+        <v>17893.830273319585</v>
       </c>
       <c r="AJ26" s="1">
         <f t="shared" si="5"/>
-        <v>4607.9520466089898</v>
+        <v>17901.246034360109</v>
       </c>
       <c r="AK26" s="1">
         <f t="shared" si="5"/>
-        <v>4630.9843824910486</v>
+        <v>17908.699896818987</v>
       </c>
       <c r="AL26" s="1">
         <f t="shared" si="5"/>
-        <v>4654.1339902568452</v>
+        <v>17916.191711507116</v>
       </c>
       <c r="AM26" s="1">
         <f t="shared" si="5"/>
-        <v>4677.4006806154612</v>
+        <v>17923.721417165041</v>
       </c>
     </row>
     <row r="27" spans="1:39" x14ac:dyDescent="0.25">
@@ -6355,64 +6355,64 @@
         <v>24614.9895</v>
       </c>
       <c r="Y27" s="1">
-        <f t="shared" ref="Y27:AM27" si="6">$X$27*Y$19/$X$19</f>
-        <v>25353.330081113923</v>
+        <f>X27</f>
+        <v>24614.9895</v>
       </c>
       <c r="Z27" s="1">
-        <f t="shared" si="6"/>
-        <v>10669.374094537761</v>
+        <f>$Y$27*Z$19/$Y$19*(1/3)+(2/3)*$Y$27</f>
+        <v>19862.87973412115</v>
       </c>
       <c r="AA27" s="1">
-        <f t="shared" si="6"/>
-        <v>4405.66840931554</v>
+        <f t="shared" ref="AA27:AM27" si="6">$Y$27*AA$19/$Y$19*(1/3)+(2/3)*$Y$27</f>
+        <v>17835.781792357582</v>
       </c>
       <c r="AB27" s="1">
         <f t="shared" si="6"/>
-        <v>4427.6967982722335</v>
+        <v>17842.910751500702</v>
       </c>
       <c r="AC27" s="1">
         <f t="shared" si="6"/>
-        <v>4449.0263974915642</v>
+        <v>17849.813564124568</v>
       </c>
       <c r="AD27" s="1">
         <f t="shared" si="6"/>
-        <v>4472.4035508416664</v>
+        <v>17857.379018477266</v>
       </c>
       <c r="AE27" s="1">
         <f t="shared" si="6"/>
-        <v>4494.6359459893101</v>
+        <v>17864.573999325519</v>
       </c>
       <c r="AF27" s="1">
         <f t="shared" si="6"/>
-        <v>4517.0324832400929</v>
+        <v>17871.822100824094</v>
       </c>
       <c r="AG27" s="1">
         <f t="shared" si="6"/>
-        <v>4539.5725058869148</v>
+        <v>17879.116637925745</v>
       </c>
       <c r="AH27" s="1">
         <f t="shared" si="6"/>
-        <v>4562.2431689469986</v>
+        <v>17886.45345366023</v>
       </c>
       <c r="AI27" s="1">
         <f t="shared" si="6"/>
-        <v>4585.0374436029961</v>
+        <v>17893.830273319585</v>
       </c>
       <c r="AJ27" s="1">
         <f t="shared" si="6"/>
-        <v>4607.9520466089898</v>
+        <v>17901.246034360109</v>
       </c>
       <c r="AK27" s="1">
         <f t="shared" si="6"/>
-        <v>4630.9843824910486</v>
+        <v>17908.699896818987</v>
       </c>
       <c r="AL27" s="1">
         <f t="shared" si="6"/>
-        <v>4654.1339902568452</v>
+        <v>17916.191711507116</v>
       </c>
       <c r="AM27" s="1">
         <f t="shared" si="6"/>
-        <v>4677.4006806154612</v>
+        <v>17923.721417165041</v>
       </c>
     </row>
     <row r="29" spans="1:39" ht="23.25" x14ac:dyDescent="0.35">
@@ -6768,8 +6768,8 @@
         <v>-207214.9895</v>
       </c>
       <c r="Y34" s="1">
-        <f>$X34*(1-Y$19/$X$30)</f>
-        <v>-205821.60272482582</v>
+        <f>X34</f>
+        <v>-207214.9895</v>
       </c>
       <c r="Z34" s="1">
         <f>$X34*(1-Z$19/$X$30)</f>
@@ -6824,7 +6824,7 @@
         <v>-206959.20421533857</v>
       </c>
       <c r="AM34" s="1">
-        <f>$X34*(1-AM$19/$X$30)</f>
+        <f t="shared" si="11"/>
         <v>-206957.92550762862</v>
       </c>
     </row>
@@ -6921,8 +6921,8 @@
         <v>-207214.9895</v>
       </c>
       <c r="Y35" s="1">
-        <f>$X35*(1-Y$19/$X$30)</f>
-        <v>-205821.60272482582</v>
+        <f>X35</f>
+        <v>-207214.9895</v>
       </c>
       <c r="Z35" s="1">
         <f>$X35*(1-Z$19/$X$30)</f>
@@ -7078,63 +7078,63 @@
       </c>
       <c r="Y38">
         <f t="shared" si="13"/>
-        <v>-180468.27264371188</v>
+        <v>-182600</v>
       </c>
       <c r="Z38">
         <f t="shared" si="13"/>
-        <v>-195959.24017525965</v>
+        <v>-186765.73453567625</v>
       </c>
       <c r="AA38">
         <f t="shared" si="13"/>
-        <v>-202567.19115833621</v>
+        <v>-189137.07777529416</v>
       </c>
       <c r="AB38">
         <f t="shared" si="13"/>
-        <v>-202543.95211713965</v>
+        <v>-189128.73816391118</v>
       </c>
       <c r="AC38">
         <f t="shared" si="13"/>
-        <v>-202521.45027027564</v>
+        <v>-189120.66310364264</v>
       </c>
       <c r="AD38">
         <f t="shared" si="13"/>
-        <v>-202496.78833831009</v>
+        <v>-189111.81287067448</v>
       </c>
       <c r="AE38">
         <f t="shared" si="13"/>
-        <v>-202473.33407900177</v>
+        <v>-189103.39602566557</v>
       </c>
       <c r="AF38">
         <f t="shared" si="13"/>
-        <v>-202449.70665654913</v>
+        <v>-189094.91703896513</v>
       </c>
       <c r="AG38">
         <f t="shared" si="13"/>
-        <v>-202425.92786292554</v>
+        <v>-189086.38373088674</v>
       </c>
       <c r="AH38">
         <f t="shared" si="13"/>
-        <v>-202402.0112490578</v>
+        <v>-189077.80096434458</v>
       </c>
       <c r="AI38">
         <f t="shared" si="13"/>
-        <v>-202377.96423005802</v>
+        <v>-189069.17140034141</v>
       </c>
       <c r="AJ38">
         <f t="shared" si="13"/>
-        <v>-202353.79026961516</v>
+        <v>-189060.49628186403</v>
       </c>
       <c r="AK38">
         <f t="shared" si="13"/>
-        <v>-202329.49210584711</v>
+        <v>-189051.77659151916</v>
       </c>
       <c r="AL38">
         <f t="shared" si="13"/>
-        <v>-202305.07022508173</v>
+        <v>-189043.01250383144</v>
       </c>
       <c r="AM38">
         <f t="shared" si="13"/>
-        <v>-202280.52482701317</v>
+        <v>-189034.20409046358</v>
       </c>
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
@@ -7229,63 +7229,63 @@
       </c>
       <c r="Y39">
         <f t="shared" si="13"/>
-        <v>-180468.27264371188</v>
+        <v>-182600</v>
       </c>
       <c r="Z39">
         <f t="shared" si="13"/>
-        <v>-195959.24017525965</v>
+        <v>-186765.73453567625</v>
       </c>
       <c r="AA39">
         <f t="shared" si="13"/>
-        <v>-202567.19115833621</v>
+        <v>-189137.07777529416</v>
       </c>
       <c r="AB39">
         <f t="shared" si="13"/>
-        <v>-202543.95211713965</v>
+        <v>-189128.73816391118</v>
       </c>
       <c r="AC39">
         <f t="shared" si="13"/>
-        <v>-202521.45027027564</v>
+        <v>-189120.66310364264</v>
       </c>
       <c r="AD39">
         <f t="shared" si="13"/>
-        <v>-202496.78833831009</v>
+        <v>-189111.81287067448</v>
       </c>
       <c r="AE39">
         <f t="shared" si="13"/>
-        <v>-202473.33407900177</v>
+        <v>-189103.39602566557</v>
       </c>
       <c r="AF39">
         <f t="shared" si="13"/>
-        <v>-202449.70665654913</v>
+        <v>-189094.91703896513</v>
       </c>
       <c r="AG39">
         <f t="shared" si="13"/>
-        <v>-202425.92786292554</v>
+        <v>-189086.38373088674</v>
       </c>
       <c r="AH39">
         <f t="shared" si="13"/>
-        <v>-202402.0112490578</v>
+        <v>-189077.80096434458</v>
       </c>
       <c r="AI39">
         <f t="shared" si="13"/>
-        <v>-202377.96423005802</v>
+        <v>-189069.17140034141</v>
       </c>
       <c r="AJ39">
         <f t="shared" si="13"/>
-        <v>-202353.79026961516</v>
+        <v>-189060.49628186403</v>
       </c>
       <c r="AK39">
         <f t="shared" si="13"/>
-        <v>-202329.49210584711</v>
+        <v>-189051.77659151916</v>
       </c>
       <c r="AL39">
         <f t="shared" si="13"/>
-        <v>-202305.07022508173</v>
+        <v>-189043.01250383144</v>
       </c>
       <c r="AM39">
         <f t="shared" si="13"/>
-        <v>-202280.52482701317</v>
+        <v>-189034.20409046358</v>
       </c>
     </row>
     <row r="42" spans="1:39" ht="28.5" x14ac:dyDescent="0.45">
@@ -7392,63 +7392,63 @@
       </c>
       <c r="Y43">
         <f t="shared" si="14"/>
-        <v>25353.330081113923</v>
+        <v>24614.9895</v>
       </c>
       <c r="Z43">
         <f t="shared" si="14"/>
-        <v>10669.374094537761</v>
+        <v>19862.87973412115</v>
       </c>
       <c r="AA43">
         <f t="shared" si="14"/>
-        <v>4405.66840931554</v>
+        <v>17835.781792357582</v>
       </c>
       <c r="AB43">
         <f t="shared" si="14"/>
-        <v>4427.6967982722335</v>
+        <v>17842.910751500702</v>
       </c>
       <c r="AC43">
         <f t="shared" si="14"/>
-        <v>4449.0263974915642</v>
+        <v>17849.813564124568</v>
       </c>
       <c r="AD43">
         <f t="shared" si="14"/>
-        <v>4472.4035508416664</v>
+        <v>17857.379018477266</v>
       </c>
       <c r="AE43">
         <f t="shared" si="14"/>
-        <v>4494.6359459893101</v>
+        <v>17864.573999325519</v>
       </c>
       <c r="AF43">
         <f t="shared" si="14"/>
-        <v>4517.0324832400929</v>
+        <v>17871.822100824094</v>
       </c>
       <c r="AG43">
         <f t="shared" si="14"/>
-        <v>4539.5725058869148</v>
+        <v>17879.116637925745</v>
       </c>
       <c r="AH43">
         <f t="shared" si="14"/>
-        <v>4562.2431689469986</v>
+        <v>17886.45345366023</v>
       </c>
       <c r="AI43">
         <f t="shared" si="14"/>
-        <v>4585.0374436029961</v>
+        <v>17893.830273319585</v>
       </c>
       <c r="AJ43">
         <f t="shared" si="14"/>
-        <v>4607.9520466089898</v>
+        <v>17901.246034360109</v>
       </c>
       <c r="AK43">
         <f t="shared" si="14"/>
-        <v>4630.9843824910486</v>
+        <v>17908.699896818987</v>
       </c>
       <c r="AL43">
         <f t="shared" si="14"/>
-        <v>4654.1339902568452</v>
+        <v>17916.191711507116</v>
       </c>
       <c r="AM43">
         <f t="shared" si="14"/>
-        <v>4677.4006806154612</v>
+        <v>17923.721417165041</v>
       </c>
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
@@ -7550,63 +7550,63 @@
       </c>
       <c r="Y44">
         <f t="shared" si="14"/>
-        <v>25353.330081113923</v>
+        <v>24614.9895</v>
       </c>
       <c r="Z44">
         <f t="shared" si="14"/>
-        <v>10669.374094537761</v>
+        <v>19862.87973412115</v>
       </c>
       <c r="AA44">
         <f t="shared" si="14"/>
-        <v>4405.66840931554</v>
+        <v>17835.781792357582</v>
       </c>
       <c r="AB44">
         <f t="shared" si="14"/>
-        <v>4427.6967982722335</v>
+        <v>17842.910751500702</v>
       </c>
       <c r="AC44">
         <f t="shared" si="14"/>
-        <v>4449.0263974915642</v>
+        <v>17849.813564124568</v>
       </c>
       <c r="AD44">
         <f t="shared" si="14"/>
-        <v>4472.4035508416664</v>
+        <v>17857.379018477266</v>
       </c>
       <c r="AE44">
         <f t="shared" si="14"/>
-        <v>4494.6359459893101</v>
+        <v>17864.573999325519</v>
       </c>
       <c r="AF44">
         <f t="shared" si="14"/>
-        <v>4517.0324832400929</v>
+        <v>17871.822100824094</v>
       </c>
       <c r="AG44">
         <f t="shared" si="14"/>
-        <v>4539.5725058869148</v>
+        <v>17879.116637925745</v>
       </c>
       <c r="AH44">
         <f t="shared" si="14"/>
-        <v>4562.2431689469986</v>
+        <v>17886.45345366023</v>
       </c>
       <c r="AI44">
         <f t="shared" si="14"/>
-        <v>4585.0374436029961</v>
+        <v>17893.830273319585</v>
       </c>
       <c r="AJ44">
         <f t="shared" si="14"/>
-        <v>4607.9520466089898</v>
+        <v>17901.246034360109</v>
       </c>
       <c r="AK44">
         <f t="shared" si="14"/>
-        <v>4630.9843824910486</v>
+        <v>17908.699896818987</v>
       </c>
       <c r="AL44">
         <f t="shared" si="14"/>
-        <v>4654.1339902568452</v>
+        <v>17916.191711507116</v>
       </c>
       <c r="AM44">
         <f t="shared" si="14"/>
-        <v>4677.4006806154612</v>
+        <v>17923.721417165041</v>
       </c>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
@@ -7708,7 +7708,7 @@
       </c>
       <c r="Y45">
         <f t="shared" si="15"/>
-        <v>-205821.60272482582</v>
+        <v>-207214.9895</v>
       </c>
       <c r="Z45">
         <f t="shared" si="15"/>
@@ -7866,7 +7866,7 @@
       </c>
       <c r="Y46">
         <f t="shared" si="15"/>
-        <v>-205821.60272482582</v>
+        <v>-207214.9895</v>
       </c>
       <c r="Z46">
         <f t="shared" si="15"/>
@@ -8024,63 +8024,63 @@
       </c>
       <c r="Y47">
         <f t="shared" si="16"/>
-        <v>-180468.27264371188</v>
+        <v>-182600</v>
       </c>
       <c r="Z47">
         <f t="shared" si="16"/>
-        <v>-195959.24017525965</v>
+        <v>-186765.73453567625</v>
       </c>
       <c r="AA47">
         <f t="shared" si="16"/>
-        <v>-202567.19115833621</v>
+        <v>-189137.07777529416</v>
       </c>
       <c r="AB47">
         <f t="shared" si="16"/>
-        <v>-202543.95211713965</v>
+        <v>-189128.73816391118</v>
       </c>
       <c r="AC47">
         <f t="shared" si="16"/>
-        <v>-202521.45027027564</v>
+        <v>-189120.66310364264</v>
       </c>
       <c r="AD47">
         <f t="shared" si="16"/>
-        <v>-202496.78833831009</v>
+        <v>-189111.81287067448</v>
       </c>
       <c r="AE47">
         <f t="shared" si="16"/>
-        <v>-202473.33407900177</v>
+        <v>-189103.39602566557</v>
       </c>
       <c r="AF47">
         <f t="shared" si="16"/>
-        <v>-202449.70665654913</v>
+        <v>-189094.91703896513</v>
       </c>
       <c r="AG47">
         <f t="shared" si="16"/>
-        <v>-202425.92786292554</v>
+        <v>-189086.38373088674</v>
       </c>
       <c r="AH47">
         <f t="shared" si="16"/>
-        <v>-202402.0112490578</v>
+        <v>-189077.80096434458</v>
       </c>
       <c r="AI47">
         <f t="shared" si="16"/>
-        <v>-202377.96423005802</v>
+        <v>-189069.17140034141</v>
       </c>
       <c r="AJ47">
         <f t="shared" si="16"/>
-        <v>-202353.79026961516</v>
+        <v>-189060.49628186403</v>
       </c>
       <c r="AK47">
         <f t="shared" si="16"/>
-        <v>-202329.49210584711</v>
+        <v>-189051.77659151916</v>
       </c>
       <c r="AL47">
         <f t="shared" si="16"/>
-        <v>-202305.07022508173</v>
+        <v>-189043.01250383144</v>
       </c>
       <c r="AM47">
         <f t="shared" si="16"/>
-        <v>-202280.52482701317</v>
+        <v>-189034.20409046358</v>
       </c>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
@@ -8182,63 +8182,63 @@
       </c>
       <c r="Y48">
         <f t="shared" si="16"/>
-        <v>-180468.27264371188</v>
+        <v>-182600</v>
       </c>
       <c r="Z48">
         <f t="shared" si="16"/>
-        <v>-195959.24017525965</v>
+        <v>-186765.73453567625</v>
       </c>
       <c r="AA48">
         <f t="shared" si="16"/>
-        <v>-202567.19115833621</v>
+        <v>-189137.07777529416</v>
       </c>
       <c r="AB48">
         <f t="shared" si="16"/>
-        <v>-202543.95211713965</v>
+        <v>-189128.73816391118</v>
       </c>
       <c r="AC48">
         <f t="shared" si="16"/>
-        <v>-202521.45027027564</v>
+        <v>-189120.66310364264</v>
       </c>
       <c r="AD48">
         <f t="shared" si="16"/>
-        <v>-202496.78833831009</v>
+        <v>-189111.81287067448</v>
       </c>
       <c r="AE48">
         <f t="shared" si="16"/>
-        <v>-202473.33407900177</v>
+        <v>-189103.39602566557</v>
       </c>
       <c r="AF48">
         <f t="shared" si="16"/>
-        <v>-202449.70665654913</v>
+        <v>-189094.91703896513</v>
       </c>
       <c r="AG48">
         <f t="shared" si="16"/>
-        <v>-202425.92786292554</v>
+        <v>-189086.38373088674</v>
       </c>
       <c r="AH48">
         <f t="shared" si="16"/>
-        <v>-202402.0112490578</v>
+        <v>-189077.80096434458</v>
       </c>
       <c r="AI48">
         <f t="shared" si="16"/>
-        <v>-202377.96423005802</v>
+        <v>-189069.17140034141</v>
       </c>
       <c r="AJ48">
         <f t="shared" si="16"/>
-        <v>-202353.79026961516</v>
+        <v>-189060.49628186403</v>
       </c>
       <c r="AK48">
         <f t="shared" si="16"/>
-        <v>-202329.49210584711</v>
+        <v>-189051.77659151916</v>
       </c>
       <c r="AL48">
         <f t="shared" si="16"/>
-        <v>-202305.07022508173</v>
+        <v>-189043.01250383144</v>
       </c>
       <c r="AM48">
         <f t="shared" si="16"/>
-        <v>-202280.52482701317</v>
+        <v>-189034.20409046358</v>
       </c>
     </row>
   </sheetData>
@@ -8250,8 +8250,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8513,63 +8513,63 @@
       </c>
       <c r="Y2">
         <f>IDN!Y43</f>
-        <v>374725.15552434477</v>
+        <v>363810.83470000001</v>
       </c>
       <c r="Z2">
         <f>IDN!Z43</f>
-        <v>290851.94404091733</v>
+        <v>336667.4002575326</v>
       </c>
       <c r="AA2">
         <f>IDN!AA43</f>
-        <v>131564.14471657577</v>
+        <v>285117.95005793608</v>
       </c>
       <c r="AB2">
         <f>IDN!AB43</f>
-        <v>132879.79383926271</v>
+        <v>285543.72647783626</v>
       </c>
       <c r="AC2">
         <f>IDN!AC43</f>
-        <v>134208.59657221258</v>
+        <v>285973.75972958462</v>
       </c>
       <c r="AD2">
         <f>IDN!AD43</f>
-        <v>135550.68591422139</v>
+        <v>286408.09285486321</v>
       </c>
       <c r="AE2">
         <f>IDN!AE43</f>
-        <v>136906.18810360983</v>
+        <v>286846.766707498</v>
       </c>
       <c r="AF2">
         <f>IDN!AF43</f>
-        <v>138275.24466730061</v>
+        <v>287289.82708908257</v>
       </c>
       <c r="AG2">
         <f>IDN!AG43</f>
-        <v>139658.01268433646</v>
+        <v>287737.32483425911</v>
       </c>
       <c r="AH2">
         <f>IDN!AH43</f>
-        <v>141054.57673898133</v>
+        <v>288189.28731657629</v>
       </c>
       <c r="AI2">
         <f>IDN!AI43</f>
-        <v>142465.13955382406</v>
+        <v>288645.78014205047</v>
       </c>
       <c r="AJ2">
         <f>IDN!AJ43</f>
-        <v>143889.7719116442</v>
+        <v>289106.82621773041</v>
       </c>
       <c r="AK2">
         <f>IDN!AK43</f>
-        <v>145328.68218574242</v>
+        <v>289572.49297834199</v>
       </c>
       <c r="AL2">
         <f>IDN!AL43</f>
-        <v>146781.96795429394</v>
+        <v>290042.81200258306</v>
       </c>
       <c r="AM2">
         <f>IDN!AM43</f>
-        <v>148249.79639635611</v>
+        <v>290517.83739370899</v>
       </c>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
@@ -8671,63 +8671,63 @@
       </c>
       <c r="Y3">
         <f>IDN!Y44</f>
-        <v>374725.15552434477</v>
+        <v>363810.83470000001</v>
       </c>
       <c r="Z3">
         <f>IDN!Z44</f>
-        <v>290851.94404091733</v>
+        <v>336667.4002575326</v>
       </c>
       <c r="AA3">
         <f>IDN!AA44</f>
-        <v>131564.14471657577</v>
+        <v>285117.95005793608</v>
       </c>
       <c r="AB3">
         <f>IDN!AB44</f>
-        <v>132879.79383926271</v>
+        <v>285543.72647783626</v>
       </c>
       <c r="AC3">
         <f>IDN!AC44</f>
-        <v>134208.59657221258</v>
+        <v>285973.75972958462</v>
       </c>
       <c r="AD3">
         <f>IDN!AD44</f>
-        <v>135550.68591422139</v>
+        <v>286408.09285486321</v>
       </c>
       <c r="AE3">
         <f>IDN!AE44</f>
-        <v>136906.18810360983</v>
+        <v>286846.766707498</v>
       </c>
       <c r="AF3">
         <f>IDN!AF44</f>
-        <v>138275.24466730061</v>
+        <v>287289.82708908257</v>
       </c>
       <c r="AG3">
         <f>IDN!AG44</f>
-        <v>139658.01268433646</v>
+        <v>287737.32483425911</v>
       </c>
       <c r="AH3">
         <f>IDN!AH44</f>
-        <v>141054.57673898133</v>
+        <v>288189.28731657629</v>
       </c>
       <c r="AI3">
         <f>IDN!AI44</f>
-        <v>142465.13955382406</v>
+        <v>288645.78014205047</v>
       </c>
       <c r="AJ3">
         <f>IDN!AJ44</f>
-        <v>143889.7719116442</v>
+        <v>289106.82621773041</v>
       </c>
       <c r="AK3">
         <f>IDN!AK44</f>
-        <v>145328.68218574242</v>
+        <v>289572.49297834199</v>
       </c>
       <c r="AL3">
         <f>IDN!AL44</f>
-        <v>146781.96795429394</v>
+        <v>290042.81200258306</v>
       </c>
       <c r="AM3">
         <f>IDN!AM44</f>
-        <v>148249.79639635611</v>
+        <v>290517.83739370899</v>
       </c>
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
@@ -8829,7 +8829,7 @@
       </c>
       <c r="Y4">
         <f>IDN!Y45</f>
-        <v>632379.27173057396</v>
+        <v>634255.83200000005</v>
       </c>
       <c r="Z4">
         <f>IDN!Z45</f>
@@ -8987,7 +8987,7 @@
       </c>
       <c r="Y5">
         <f>IDN!Y46</f>
-        <v>632379.27173057396</v>
+        <v>634255.83200000005</v>
       </c>
       <c r="Z5">
         <f>IDN!Z46</f>
@@ -9145,63 +9145,63 @@
       </c>
       <c r="Y6">
         <f>IDN!Y47</f>
-        <v>1007104.4272549187</v>
+        <v>998066.66670000006</v>
       </c>
       <c r="Z6">
         <f>IDN!Z47</f>
-        <v>923651.23864430515</v>
+        <v>969466.69486092043</v>
       </c>
       <c r="AA6">
         <f>IDN!AA47</f>
-        <v>765161.12570746569</v>
+        <v>918714.93104882608</v>
       </c>
       <c r="AB6">
         <f>IDN!AB47</f>
-        <v>766470.18628162378</v>
+        <v>919134.11892019736</v>
       </c>
       <c r="AC6">
         <f>IDN!AC47</f>
-        <v>767792.3345949871</v>
+        <v>919557.49775235914</v>
       </c>
       <c r="AD6">
         <f>IDN!AD47</f>
-        <v>769127.70298031578</v>
+        <v>919985.10992095759</v>
       </c>
       <c r="AE6">
         <f>IDN!AE47</f>
-        <v>770476.41704375041</v>
+        <v>920416.99564763857</v>
       </c>
       <c r="AF6">
         <f>IDN!AF47</f>
-        <v>771838.61760347104</v>
+        <v>920853.200025253</v>
       </c>
       <c r="AG6">
         <f>IDN!AG47</f>
-        <v>773214.46095189475</v>
+        <v>921293.77310181747</v>
       </c>
       <c r="AH6">
         <f>IDN!AH47</f>
-        <v>774604.03124970198</v>
+        <v>921738.74182729702</v>
       </c>
       <c r="AI6">
         <f>IDN!AI47</f>
-        <v>776007.53020428133</v>
+        <v>922188.17079250771</v>
       </c>
       <c r="AJ6">
         <f>IDN!AJ47</f>
-        <v>777425.02824394358</v>
+        <v>922642.08255002985</v>
       </c>
       <c r="AK6">
         <f>IDN!AK47</f>
-        <v>778856.73269849166</v>
+        <v>923100.54349109123</v>
       </c>
       <c r="AL6">
         <f>IDN!AL47</f>
-        <v>780302.74065744539</v>
+        <v>923563.58470573451</v>
       </c>
       <c r="AM6">
         <f>IDN!AM47</f>
-        <v>781763.21846265788</v>
+        <v>924031.2594600108</v>
       </c>
     </row>
     <row r="7" spans="1:39" x14ac:dyDescent="0.25">
@@ -9303,63 +9303,63 @@
       </c>
       <c r="Y7">
         <f>IDN!Y48</f>
-        <v>1007104.4272549187</v>
+        <v>998066.66670000006</v>
       </c>
       <c r="Z7">
         <f>IDN!Z48</f>
-        <v>923651.23864430515</v>
+        <v>969466.69486092043</v>
       </c>
       <c r="AA7">
         <f>IDN!AA48</f>
-        <v>765161.12570746569</v>
+        <v>918714.93104882608</v>
       </c>
       <c r="AB7">
         <f>IDN!AB48</f>
-        <v>766470.18628162378</v>
+        <v>919134.11892019736</v>
       </c>
       <c r="AC7">
         <f>IDN!AC48</f>
-        <v>767792.3345949871</v>
+        <v>919557.49775235914</v>
       </c>
       <c r="AD7">
         <f>IDN!AD48</f>
-        <v>769127.70298031578</v>
+        <v>919985.10992095759</v>
       </c>
       <c r="AE7">
         <f>IDN!AE48</f>
-        <v>770476.41704375041</v>
+        <v>920416.99564763857</v>
       </c>
       <c r="AF7">
         <f>IDN!AF48</f>
-        <v>771838.61760347104</v>
+        <v>920853.200025253</v>
       </c>
       <c r="AG7">
         <f>IDN!AG48</f>
-        <v>773214.46095189475</v>
+        <v>921293.77310181747</v>
       </c>
       <c r="AH7">
         <f>IDN!AH48</f>
-        <v>774604.03124970198</v>
+        <v>921738.74182729702</v>
       </c>
       <c r="AI7">
         <f>IDN!AI48</f>
-        <v>776007.53020428133</v>
+        <v>922188.17079250771</v>
       </c>
       <c r="AJ7">
         <f>IDN!AJ48</f>
-        <v>777425.02824394358</v>
+        <v>922642.08255002985</v>
       </c>
       <c r="AK7">
         <f>IDN!AK48</f>
-        <v>778856.73269849166</v>
+        <v>923100.54349109123</v>
       </c>
       <c r="AL7">
         <f>IDN!AL48</f>
-        <v>780302.74065744539</v>
+        <v>923563.58470573451</v>
       </c>
       <c r="AM7">
         <f>IDN!AM48</f>
-        <v>781763.21846265788</v>
+        <v>924031.2594600108</v>
       </c>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
@@ -9461,63 +9461,63 @@
       </c>
       <c r="Y8">
         <f>MYS!Y43</f>
-        <v>25353.330081113923</v>
+        <v>24614.9895</v>
       </c>
       <c r="Z8">
         <f>MYS!Z43</f>
-        <v>10669.374094537761</v>
+        <v>19862.87973412115</v>
       </c>
       <c r="AA8">
         <f>MYS!AA43</f>
-        <v>4405.66840931554</v>
+        <v>17835.781792357582</v>
       </c>
       <c r="AB8">
         <f>MYS!AB43</f>
-        <v>4427.6967982722335</v>
+        <v>17842.910751500702</v>
       </c>
       <c r="AC8">
         <f>MYS!AC43</f>
-        <v>4449.0263974915642</v>
+        <v>17849.813564124568</v>
       </c>
       <c r="AD8">
         <f>MYS!AD43</f>
-        <v>4472.4035508416664</v>
+        <v>17857.379018477266</v>
       </c>
       <c r="AE8">
         <f>MYS!AE43</f>
-        <v>4494.6359459893101</v>
+        <v>17864.573999325519</v>
       </c>
       <c r="AF8">
         <f>MYS!AF43</f>
-        <v>4517.0324832400929</v>
+        <v>17871.822100824094</v>
       </c>
       <c r="AG8">
         <f>MYS!AG43</f>
-        <v>4539.5725058869148</v>
+        <v>17879.116637925745</v>
       </c>
       <c r="AH8">
         <f>MYS!AH43</f>
-        <v>4562.2431689469986</v>
+        <v>17886.45345366023</v>
       </c>
       <c r="AI8">
         <f>MYS!AI43</f>
-        <v>4585.0374436029961</v>
+        <v>17893.830273319585</v>
       </c>
       <c r="AJ8">
         <f>MYS!AJ43</f>
-        <v>4607.9520466089898</v>
+        <v>17901.246034360109</v>
       </c>
       <c r="AK8">
         <f>MYS!AK43</f>
-        <v>4630.9843824910486</v>
+        <v>17908.699896818987</v>
       </c>
       <c r="AL8">
         <f>MYS!AL43</f>
-        <v>4654.1339902568452</v>
+        <v>17916.191711507116</v>
       </c>
       <c r="AM8">
         <f>MYS!AM43</f>
-        <v>4677.4006806154612</v>
+        <v>17923.721417165041</v>
       </c>
     </row>
     <row r="9" spans="1:39" x14ac:dyDescent="0.25">
@@ -9619,63 +9619,63 @@
       </c>
       <c r="Y9">
         <f>MYS!Y44</f>
-        <v>25353.330081113923</v>
+        <v>24614.9895</v>
       </c>
       <c r="Z9">
         <f>MYS!Z44</f>
-        <v>10669.374094537761</v>
+        <v>19862.87973412115</v>
       </c>
       <c r="AA9">
         <f>MYS!AA44</f>
-        <v>4405.66840931554</v>
+        <v>17835.781792357582</v>
       </c>
       <c r="AB9">
         <f>MYS!AB44</f>
-        <v>4427.6967982722335</v>
+        <v>17842.910751500702</v>
       </c>
       <c r="AC9">
         <f>MYS!AC44</f>
-        <v>4449.0263974915642</v>
+        <v>17849.813564124568</v>
       </c>
       <c r="AD9">
         <f>MYS!AD44</f>
-        <v>4472.4035508416664</v>
+        <v>17857.379018477266</v>
       </c>
       <c r="AE9">
         <f>MYS!AE44</f>
-        <v>4494.6359459893101</v>
+        <v>17864.573999325519</v>
       </c>
       <c r="AF9">
         <f>MYS!AF44</f>
-        <v>4517.0324832400929</v>
+        <v>17871.822100824094</v>
       </c>
       <c r="AG9">
         <f>MYS!AG44</f>
-        <v>4539.5725058869148</v>
+        <v>17879.116637925745</v>
       </c>
       <c r="AH9">
         <f>MYS!AH44</f>
-        <v>4562.2431689469986</v>
+        <v>17886.45345366023</v>
       </c>
       <c r="AI9">
         <f>MYS!AI44</f>
-        <v>4585.0374436029961</v>
+        <v>17893.830273319585</v>
       </c>
       <c r="AJ9">
         <f>MYS!AJ44</f>
-        <v>4607.9520466089898</v>
+        <v>17901.246034360109</v>
       </c>
       <c r="AK9">
         <f>MYS!AK44</f>
-        <v>4630.9843824910486</v>
+        <v>17908.699896818987</v>
       </c>
       <c r="AL9">
         <f>MYS!AL44</f>
-        <v>4654.1339902568452</v>
+        <v>17916.191711507116</v>
       </c>
       <c r="AM9">
         <f>MYS!AM44</f>
-        <v>4677.4006806154612</v>
+        <v>17923.721417165041</v>
       </c>
     </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.25">
@@ -9777,7 +9777,7 @@
       </c>
       <c r="Y10">
         <f>MYS!Y45</f>
-        <v>-205821.60272482582</v>
+        <v>-207214.9895</v>
       </c>
       <c r="Z10">
         <f>MYS!Z45</f>
@@ -9935,7 +9935,7 @@
       </c>
       <c r="Y11">
         <f>MYS!Y46</f>
-        <v>-205821.60272482582</v>
+        <v>-207214.9895</v>
       </c>
       <c r="Z11">
         <f>MYS!Z46</f>
@@ -10093,63 +10093,63 @@
       </c>
       <c r="Y12">
         <f>MYS!Y47</f>
-        <v>-180468.27264371188</v>
+        <v>-182600</v>
       </c>
       <c r="Z12">
         <f>MYS!Z47</f>
-        <v>-195959.24017525965</v>
+        <v>-186765.73453567625</v>
       </c>
       <c r="AA12">
         <f>MYS!AA47</f>
-        <v>-202567.19115833621</v>
+        <v>-189137.07777529416</v>
       </c>
       <c r="AB12">
         <f>MYS!AB47</f>
-        <v>-202543.95211713965</v>
+        <v>-189128.73816391118</v>
       </c>
       <c r="AC12">
         <f>MYS!AC47</f>
-        <v>-202521.45027027564</v>
+        <v>-189120.66310364264</v>
       </c>
       <c r="AD12">
         <f>MYS!AD47</f>
-        <v>-202496.78833831009</v>
+        <v>-189111.81287067448</v>
       </c>
       <c r="AE12">
         <f>MYS!AE47</f>
-        <v>-202473.33407900177</v>
+        <v>-189103.39602566557</v>
       </c>
       <c r="AF12">
         <f>MYS!AF47</f>
-        <v>-202449.70665654913</v>
+        <v>-189094.91703896513</v>
       </c>
       <c r="AG12">
         <f>MYS!AG47</f>
-        <v>-202425.92786292554</v>
+        <v>-189086.38373088674</v>
       </c>
       <c r="AH12">
         <f>MYS!AH47</f>
-        <v>-202402.0112490578</v>
+        <v>-189077.80096434458</v>
       </c>
       <c r="AI12">
         <f>MYS!AI47</f>
-        <v>-202377.96423005802</v>
+        <v>-189069.17140034141</v>
       </c>
       <c r="AJ12">
         <f>MYS!AJ47</f>
-        <v>-202353.79026961516</v>
+        <v>-189060.49628186403</v>
       </c>
       <c r="AK12">
         <f>MYS!AK47</f>
-        <v>-202329.49210584711</v>
+        <v>-189051.77659151916</v>
       </c>
       <c r="AL12">
         <f>MYS!AL47</f>
-        <v>-202305.07022508173</v>
+        <v>-189043.01250383144</v>
       </c>
       <c r="AM12">
         <f>MYS!AM47</f>
-        <v>-202280.52482701317</v>
+        <v>-189034.20409046358</v>
       </c>
     </row>
     <row r="13" spans="1:39" x14ac:dyDescent="0.25">
@@ -10251,63 +10251,63 @@
       </c>
       <c r="Y13">
         <f>MYS!Y48</f>
-        <v>-180468.27264371188</v>
+        <v>-182600</v>
       </c>
       <c r="Z13">
         <f>MYS!Z48</f>
-        <v>-195959.24017525965</v>
+        <v>-186765.73453567625</v>
       </c>
       <c r="AA13">
         <f>MYS!AA48</f>
-        <v>-202567.19115833621</v>
+        <v>-189137.07777529416</v>
       </c>
       <c r="AB13">
         <f>MYS!AB48</f>
-        <v>-202543.95211713965</v>
+        <v>-189128.73816391118</v>
       </c>
       <c r="AC13">
         <f>MYS!AC48</f>
-        <v>-202521.45027027564</v>
+        <v>-189120.66310364264</v>
       </c>
       <c r="AD13">
         <f>MYS!AD48</f>
-        <v>-202496.78833831009</v>
+        <v>-189111.81287067448</v>
       </c>
       <c r="AE13">
         <f>MYS!AE48</f>
-        <v>-202473.33407900177</v>
+        <v>-189103.39602566557</v>
       </c>
       <c r="AF13">
         <f>MYS!AF48</f>
-        <v>-202449.70665654913</v>
+        <v>-189094.91703896513</v>
       </c>
       <c r="AG13">
         <f>MYS!AG48</f>
-        <v>-202425.92786292554</v>
+        <v>-189086.38373088674</v>
       </c>
       <c r="AH13">
         <f>MYS!AH48</f>
-        <v>-202402.0112490578</v>
+        <v>-189077.80096434458</v>
       </c>
       <c r="AI13">
         <f>MYS!AI48</f>
-        <v>-202377.96423005802</v>
+        <v>-189069.17140034141</v>
       </c>
       <c r="AJ13">
         <f>MYS!AJ48</f>
-        <v>-202353.79026961516</v>
+        <v>-189060.49628186403</v>
       </c>
       <c r="AK13">
         <f>MYS!AK48</f>
-        <v>-202329.49210584711</v>
+        <v>-189051.77659151916</v>
       </c>
       <c r="AL13">
         <f>MYS!AL48</f>
-        <v>-202305.07022508173</v>
+        <v>-189043.01250383144</v>
       </c>
       <c r="AM13">
         <f>MYS!AM48</f>
-        <v>-202280.52482701317</v>
+        <v>-189034.20409046358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>